<commit_message>
Added -TTest and FlowContour
</commit_message>
<xml_diff>
--- a/FeatureNames.xlsx
+++ b/FeatureNames.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Georgia Tech\MLB Fall 2015\MLB_Flow\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>Tube1_FSC_mean</t>
   </si>
@@ -52,14 +57,148 @@
   </si>
   <si>
     <t>IgG1-PC5_stdev</t>
+  </si>
+  <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t>FSC</t>
+  </si>
+  <si>
+    <t>SSC</t>
+  </si>
+  <si>
+    <t>FL1</t>
+  </si>
+  <si>
+    <t>FL2</t>
+  </si>
+  <si>
+    <t>FL3</t>
+  </si>
+  <si>
+    <t>FL4</t>
+  </si>
+  <si>
+    <t>FL5</t>
+  </si>
+  <si>
+    <t>CD45-ECD</t>
+  </si>
+  <si>
+    <t>NS1</t>
+  </si>
+  <si>
+    <t>NS2</t>
+  </si>
+  <si>
+    <t>NS3</t>
+  </si>
+  <si>
+    <t>NS4</t>
+  </si>
+  <si>
+    <t>NS5</t>
+  </si>
+  <si>
+    <t>IgG1-FITC</t>
+  </si>
+  <si>
+    <t>Kappa-FIT</t>
+  </si>
+  <si>
+    <t>CD7-FITC</t>
+  </si>
+  <si>
+    <t>CD15-FITC</t>
+  </si>
+  <si>
+    <t>CD14-FITC</t>
+  </si>
+  <si>
+    <t>HLA-DR-FITC</t>
+  </si>
+  <si>
+    <t>CD5-FITC</t>
+  </si>
+  <si>
+    <t>Lambda-PE</t>
+  </si>
+  <si>
+    <t>IgG1-PE</t>
+  </si>
+  <si>
+    <t>CD4-PE</t>
+  </si>
+  <si>
+    <t>CD13-PE</t>
+  </si>
+  <si>
+    <t>CD11c-PE</t>
+  </si>
+  <si>
+    <t>CD117-PE</t>
+  </si>
+  <si>
+    <t>CD19-PE</t>
+  </si>
+  <si>
+    <t>IgG1-PC5</t>
+  </si>
+  <si>
+    <t>CD19-PC5</t>
+  </si>
+  <si>
+    <t>CD8-PC5</t>
+  </si>
+  <si>
+    <t>CD16-PC5</t>
+  </si>
+  <si>
+    <t>CD64-PC5</t>
+  </si>
+  <si>
+    <t>CD34-PC5</t>
+  </si>
+  <si>
+    <t>CD3-PC5</t>
+  </si>
+  <si>
+    <t>IgG1-PC7</t>
+  </si>
+  <si>
+    <t>CD20-PC7</t>
+  </si>
+  <si>
+    <t>CD2-PC7</t>
+  </si>
+  <si>
+    <t>CD56-PC7</t>
+  </si>
+  <si>
+    <t>CD33-PC7</t>
+  </si>
+  <si>
+    <t>CD38-PC7</t>
+  </si>
+  <si>
+    <t>CD10-PC7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,8 +226,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,6 +238,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -146,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -181,7 +324,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,79 +533,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>